<commit_message>
updated timesheets for 9/20/2021
</commit_message>
<xml_diff>
--- a/Admin/Ara Folder/Timesheet_9-13_9-19.xlsx
+++ b/Admin/Ara Folder/Timesheet_9-13_9-19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Desktop\Ara Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Desktop\SeniorDesignProject\Admin\Ara Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0A20EDF-7E22-4202-B28C-9BA9AB1379A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B971AE-B1CA-4A25-A866-3F88D0599E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,7 +724,9 @@
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9">
+        <v>1.25</v>
+      </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -733,7 +735,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I15" si="0">SUM(B6:H6)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J6" s="7"/>
     </row>
@@ -900,7 +902,7 @@
       </c>
       <c r="B16" s="11">
         <f t="shared" ref="B16:I16" si="1">SUM(B6:B15)</f>
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="C16" s="11">
         <f t="shared" si="1"/>
@@ -928,7 +930,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3.25</v>
       </c>
       <c r="J16" s="12"/>
     </row>

</xml_diff>